<commit_message>
Perbaiki impor data suplemen
</commit_message>
<xml_diff>
--- a/assets/import/format_impor_suplemen.xlsx
+++ b/assets/import/format_impor_suplemen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\OpenSID\assets\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OpenDesa\OpenSID\assets\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3341EE6-CCB9-4B3E-91E3-F82AF12EF55D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0997A0BE-D18D-4C21-A18F-0887E27D123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Peserta" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Peserta</t>
   </si>
@@ -46,43 +46,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>2. Kolom Peserta (A)  wajib di isi</t>
-  </si>
-  <si>
-    <t>Nama</t>
-  </si>
-  <si>
-    <t>Tempat Lahir</t>
-  </si>
-  <si>
-    <t>Tanggal Lahir</t>
-  </si>
-  <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>AHLUL</t>
-  </si>
-  <si>
-    <t>MANGSIT</t>
-  </si>
-  <si>
-    <t>1970-05-20</t>
-  </si>
-  <si>
-    <t>RT 004 RW - Dusun Mangsit</t>
-  </si>
-  <si>
-    <t>AHMAD HABIB</t>
-  </si>
-  <si>
-    <t>1990-01-03</t>
-  </si>
-  <si>
-    <t>3. Kolom (B, C, D, E) diambil dari database kependudukan</t>
-  </si>
-  <si>
-    <t>4. Kolom (F) opsional</t>
+    <t>2. Kolom Peserta (A, B)  wajib di isi</t>
   </si>
 </sst>
 </file>
@@ -165,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -186,10 +150,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -507,141 +467,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.25" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.875" customWidth="1"/>
-    <col min="6" max="6" width="18.25" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>